<commit_message>
two more days data
</commit_message>
<xml_diff>
--- a/va_facility_data_2025-02-20/A.K. Baker VA Clinic - Facility Data.xlsx"; filename*=UTF-8''A.K.%20Baker%20VA%20Clinic%20-%20Facility%20Data.xlsx
+++ b/va_facility_data_2025-02-20/A.K. Baker VA Clinic - Facility Data.xlsx"; filename*=UTF-8''A.K.%20Baker%20VA%20Clinic%20-%20Facility%20Data.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Wait Times" sheetId="1" r:id="R18e7a3b9f3514f99b9a1fab06f2b8fec"/>
-    <x:sheet name="Satisfaction with Care" sheetId="2" r:id="R4367fa18465c435d806f1ffe55fda5ba"/>
-    <x:sheet name="Outpatient Score" sheetId="3" r:id="Rfdfd8f99afb348ac915e58f6265aa183"/>
+    <x:sheet name="Wait Times" sheetId="1" r:id="R9da04d239b5e4f78b9b81bf8836f1f87"/>
+    <x:sheet name="Satisfaction with Care" sheetId="2" r:id="R336542e7d1c34736bfeb3639526e0d53"/>
+    <x:sheet name="Outpatient Score" sheetId="3" r:id="R26ecd4aca8834c3daa1246c4904e35d3"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>